<commit_message>
Added Excel Sheet Model class and using dynamic sendBody to Jdbc Bean for each row
</commit_message>
<xml_diff>
--- a/data/sampledata.xlsx
+++ b/data/sampledata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>FirstName</t>
   </si>
@@ -43,12 +43,40 @@
   </si>
   <si>
     <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>MemberID</t>
+  </si>
+  <si>
+    <t>VisitingDate</t>
+  </si>
+  <si>
+    <t>ExerciseZone</t>
+  </si>
+  <si>
+    <t>Track</t>
+  </si>
+  <si>
+    <t>HeavyLifting</t>
+  </si>
+  <si>
+    <t>5/14/2017</t>
+  </si>
+  <si>
+    <t>6/19/2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/dd/yy;@"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,9 +114,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -98,6 +132,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -146,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -181,7 +218,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,18 +427,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,8 +449,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -422,8 +463,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="2">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -432,6 +476,9 @@
       </c>
       <c r="C3" t="s">
         <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -442,13 +489,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>